<commit_message>
Calculated and plotted temp vs alpha-helix
</commit_message>
<xml_diff>
--- a/EAAAK/Helixvstemperature.xlsx
+++ b/EAAAK/Helixvstemperature.xlsx
@@ -185,7 +185,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -240,10 +240,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$C$2:$C$6</c:f>
+                <c:f>Sheet1!$C$2:$C$7</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
+                  <c:ptCount val="6"/>
                   <c:pt idx="0">
                     <c:v>0.0745652790066</c:v>
                   </c:pt>
@@ -254,9 +254,12 @@
                     <c:v>0.0876410149416</c:v>
                   </c:pt>
                   <c:pt idx="3">
+                    <c:v>0.0752455014344</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
                     <c:v>0.116189973451</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>0.020939554211</c:v>
                   </c:pt>
                 </c:numCache>
@@ -264,10 +267,10 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$C$2:$C$6</c:f>
+                <c:f>Sheet1!$C$2:$C$7</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
+                  <c:ptCount val="6"/>
                   <c:pt idx="0">
                     <c:v>0.0745652790066</c:v>
                   </c:pt>
@@ -278,9 +281,12 @@
                     <c:v>0.0876410149416</c:v>
                   </c:pt>
                   <c:pt idx="3">
+                    <c:v>0.0752455014344</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
                     <c:v>0.116189973451</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>0.020939554211</c:v>
                   </c:pt>
                 </c:numCache>
@@ -289,10 +295,10 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -303,9 +309,12 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
@@ -313,10 +322,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.70345</c:v>
                 </c:pt>
@@ -327,9 +336,12 @@
                   <c:v>0.597883333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.475758333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.342241666667</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.0131416666667</c:v>
                 </c:pt>
               </c:numCache>
@@ -337,11 +349,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="34523032"/>
-        <c:axId val="84074355"/>
+        <c:axId val="48159958"/>
+        <c:axId val="17693851"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="34523032"/>
+        <c:axId val="48159958"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -376,12 +388,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84074355"/>
+        <c:crossAx val="17693851"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84074355"/>
+        <c:axId val="17693851"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -425,7 +437,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34523032"/>
+        <c:crossAx val="48159958"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -492,10 +504,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
+      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -549,23 +561,34 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.342241666667</v>
+        <v>0.475758333333</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.116189973451</v>
+        <v>0.0752455014344</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.342241666667</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.116189973451</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B7" s="0" t="n">
         <v>0.0131416666667</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C7" s="0" t="n">
         <v>0.020939554211</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 150C for EAAAK
</commit_message>
<xml_diff>
--- a/EAAAK/Helixvstemperature.xlsx
+++ b/EAAAK/Helixvstemperature.xlsx
@@ -62,6 +62,7 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -185,7 +186,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -226,6 +227,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -240,10 +242,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$C$2:$C$7</c:f>
+                <c:f>Sheet1!$C$2:$C$8</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="6"/>
+                  <c:ptCount val="7"/>
                   <c:pt idx="0">
                     <c:v>0.0745652790066</c:v>
                   </c:pt>
@@ -260,6 +262,9 @@
                     <c:v>0.116189973451</c:v>
                   </c:pt>
                   <c:pt idx="5">
+                    <c:v>0.0577740804773</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
                     <c:v>0.020939554211</c:v>
                   </c:pt>
                 </c:numCache>
@@ -267,10 +272,10 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$C$2:$C$7</c:f>
+                <c:f>Sheet1!$C$2:$C$8</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="6"/>
+                  <c:ptCount val="7"/>
                   <c:pt idx="0">
                     <c:v>0.0745652790066</c:v>
                   </c:pt>
@@ -287,6 +292,9 @@
                     <c:v>0.116189973451</c:v>
                   </c:pt>
                   <c:pt idx="5">
+                    <c:v>0.0577740804773</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
                     <c:v>0.020939554211</c:v>
                   </c:pt>
                 </c:numCache>
@@ -295,10 +303,10 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -315,6 +323,9 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
@@ -322,10 +333,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.70345</c:v>
                 </c:pt>
@@ -342,6 +353,9 @@
                   <c:v>0.342241666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0.070375</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.0131416666667</c:v>
                 </c:pt>
               </c:numCache>
@@ -349,17 +363,17 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="48159958"/>
-        <c:axId val="17693851"/>
+        <c:axId val="57216534"/>
+        <c:axId val="6860956"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48159958"/>
+        <c:axId val="57216534"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -388,12 +402,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17693851"/>
+        <c:crossAx val="6860956"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="17693851"/>
+        <c:axId val="6860956"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -408,7 +422,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -437,7 +451,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48159958"/>
+        <c:crossAx val="57216534"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -469,14 +483,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>553320</xdr:colOff>
+      <xdr:colOff>553680</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>57240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>158040</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:colOff>157680</xdr:colOff>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>38160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
@@ -485,8 +499,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2953440" y="57240"/>
-        <a:ext cx="6805800" cy="3557160"/>
+        <a:off x="2896560" y="57240"/>
+        <a:ext cx="6633720" cy="3719520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -504,16 +518,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -583,12 +594,23 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.070375</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.0577740804773</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B8" s="0" t="n">
         <v>0.0131416666667</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C8" s="0" t="n">
         <v>0.020939554211</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 125 and calculated KDE & heatmaps
</commit_message>
<xml_diff>
--- a/EAAAK/Helixvstemperature.xlsx
+++ b/EAAAK/Helixvstemperature.xlsx
@@ -109,8 +109,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -242,10 +246,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$C$2:$C$8</c:f>
+                <c:f>Sheet1!$C$2:$C$9</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="7"/>
+                  <c:ptCount val="8"/>
                   <c:pt idx="0">
                     <c:v>0.0745652790066</c:v>
                   </c:pt>
@@ -262,9 +266,12 @@
                     <c:v>0.116189973451</c:v>
                   </c:pt>
                   <c:pt idx="5">
+                    <c:v>0.0683777695966</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
                     <c:v>0.0577740804773</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>0.020939554211</c:v>
                   </c:pt>
                 </c:numCache>
@@ -272,10 +279,10 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$C$2:$C$8</c:f>
+                <c:f>Sheet1!$C$2:$C$9</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="7"/>
+                  <c:ptCount val="8"/>
                   <c:pt idx="0">
                     <c:v>0.0745652790066</c:v>
                   </c:pt>
@@ -292,9 +299,12 @@
                     <c:v>0.116189973451</c:v>
                   </c:pt>
                   <c:pt idx="5">
+                    <c:v>0.0683777695966</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
                     <c:v>0.0577740804773</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>0.020939554211</c:v>
                   </c:pt>
                 </c:numCache>
@@ -303,10 +313,10 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -323,9 +333,12 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
@@ -333,10 +346,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:f>Sheet1!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.70345</c:v>
                 </c:pt>
@@ -353,9 +366,12 @@
                   <c:v>0.342241666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0.145125</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.070375</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.0131416666667</c:v>
                 </c:pt>
               </c:numCache>
@@ -363,11 +379,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="57216534"/>
-        <c:axId val="6860956"/>
+        <c:axId val="80086843"/>
+        <c:axId val="16724249"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57216534"/>
+        <c:axId val="80086843"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -402,12 +418,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6860956"/>
+        <c:crossAx val="16724249"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="6860956"/>
+        <c:axId val="16724249"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -451,7 +467,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57216534"/>
+        <c:crossAx val="80086843"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -483,15 +499,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>553680</xdr:colOff>
+      <xdr:colOff>554040</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>57240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>157680</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -499,8 +515,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2896560" y="57240"/>
-        <a:ext cx="6633720" cy="3719520"/>
+        <a:off x="2354040" y="57240"/>
+        <a:ext cx="5004360" cy="3881880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -518,99 +534,113 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.70345</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>0.0745652790066</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.700366666667</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>0.0942124608413</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>0.597883333333</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>0.0876410149416</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.475758333333</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>0.0752455014344</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>0.342241666667</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>0.116189973451</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.145125</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.0683777695966</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>0.070375</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>0.0577740804773</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>0.0131416666667</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>0.020939554211</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added 37 and mutant 200 Mark
</commit_message>
<xml_diff>
--- a/EAAAK/Helixvstemperature.xlsx
+++ b/EAAAK/Helixvstemperature.xlsx
@@ -190,7 +190,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -246,10 +246,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$C$2:$C$9</c:f>
+                <c:f>Sheet1!$C$2:$C$10</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="8"/>
+                  <c:ptCount val="9"/>
                   <c:pt idx="0">
                     <c:v>0.0745652790066</c:v>
                   </c:pt>
@@ -257,21 +257,24 @@
                     <c:v>0.0942124608413</c:v>
                   </c:pt>
                   <c:pt idx="2">
+                    <c:v>0.076166961615</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
                     <c:v>0.0876410149416</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>0.0752455014344</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>0.116189973451</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>0.0683777695966</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>0.0577740804773</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="8">
                     <c:v>0.020939554211</c:v>
                   </c:pt>
                 </c:numCache>
@@ -279,10 +282,10 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$C$2:$C$9</c:f>
+                <c:f>Sheet1!$C$2:$C$10</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="8"/>
+                  <c:ptCount val="9"/>
                   <c:pt idx="0">
                     <c:v>0.0745652790066</c:v>
                   </c:pt>
@@ -290,21 +293,24 @@
                     <c:v>0.0942124608413</c:v>
                   </c:pt>
                   <c:pt idx="2">
+                    <c:v>0.076166961615</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
                     <c:v>0.0876410149416</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>0.0752455014344</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>0.116189973451</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>0.0683777695966</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>0.0577740804773</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="8">
                     <c:v>0.020939554211</c:v>
                   </c:pt>
                 </c:numCache>
@@ -313,10 +319,10 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -324,21 +330,24 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>125</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
@@ -346,10 +355,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:f>Sheet1!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.70345</c:v>
                 </c:pt>
@@ -357,21 +366,24 @@
                   <c:v>0.700366666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.640191666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.597883333333</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.475758333333</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.342241666667</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.145125</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.070375</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.0131416666667</c:v>
                 </c:pt>
               </c:numCache>
@@ -379,11 +391,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="49964743"/>
-        <c:axId val="76949186"/>
+        <c:axId val="32761163"/>
+        <c:axId val="50528172"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49964743"/>
+        <c:axId val="32761163"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -418,12 +430,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76949186"/>
+        <c:crossAx val="50528172"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76949186"/>
+        <c:axId val="50528172"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -467,7 +479,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49964743"/>
+        <c:crossAx val="32761163"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -499,14 +511,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>554040</xdr:colOff>
+      <xdr:colOff>554400</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>57240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>157320</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>37440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
@@ -515,8 +527,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2325600" y="57240"/>
-        <a:ext cx="4918320" cy="3881520"/>
+        <a:off x="2297160" y="57240"/>
+        <a:ext cx="4832280" cy="4043880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -534,15 +546,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="A7:C7"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -580,67 +592,78 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>0.597883333333</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>0.0876410149416</v>
+        <v>37</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.640191666667</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.076166961615</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>0.475758333333</v>
+        <v>0.597883333333</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>0.0752455014344</v>
+        <v>0.0876410149416</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>0.342241666667</v>
+        <v>0.475758333333</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>0.116189973451</v>
+        <v>0.0752455014344</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>125</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>0.145125</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>0.0683777695966</v>
+        <v>100</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>0.342241666667</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>0.116189973451</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>0.070375</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>0.0577740804773</v>
+        <v>125</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.145125</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.0683777695966</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>0.070375</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>0.0577740804773</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B10" s="1" t="n">
         <v>0.0131416666667</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C10" s="1" t="n">
         <v>0.020939554211</v>
       </c>
     </row>

</xml_diff>